<commit_message>
feat: change PFAS selection criteria
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PFAS_ng_gdw/1.BMF_diet_PFAS_ng_gdw_censored.xlsx
+++ b/inst/results/BMF_computation_PFAS_ng_gdw/1.BMF_diet_PFAS_ng_gdw_censored.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,7 +412,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6:2 FTSA</t>
+          <t>8:2 FTSA</t>
         </is>
       </c>
       <c r="B2">
@@ -422,16 +422,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="E2">
-        <v>1.16</v>
+        <v>0.04</v>
       </c>
       <c r="F2">
-        <v>1.87</v>
+        <v>0.1</v>
       </c>
       <c r="G2">
-        <v>3.26</v>
+        <v>0.2</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -440,323 +440,321 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>8:2 FTSA</t>
+          <t>Br-PFOS</t>
         </is>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1.41</v>
       </c>
       <c r="D3">
-        <v>0.13</v>
+        <v>2.79</v>
       </c>
       <c r="E3">
-        <v>0.04</v>
+        <v>0.14</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>0.39</v>
       </c>
       <c r="G3">
-        <v>0.2</v>
+        <v>0.86</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>3.61</v>
       </c>
       <c r="J3">
-        <v>3.18</v>
+        <v>20.13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Br-PFOS</t>
+          <t>EtFOSAA</t>
         </is>
       </c>
       <c r="B4">
-        <v>0.9399999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="C4">
-        <v>1.41</v>
+        <v>0.22</v>
       </c>
       <c r="D4">
-        <v>2.79</v>
+        <v>0.37</v>
       </c>
       <c r="E4">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="F4">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="G4">
-        <v>0.86</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="H4">
-        <v>1.1</v>
+        <v>0.12</v>
       </c>
       <c r="I4">
-        <v>3.61</v>
+        <v>0.62</v>
       </c>
       <c r="J4">
-        <v>20.13</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EtFOSAA</t>
+          <t>FOSA</t>
         </is>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="C5">
-        <v>0.22</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
-        <v>0.37</v>
+        <v>0.92</v>
       </c>
       <c r="E5">
+        <v>2.07</v>
+      </c>
+      <c r="F5">
+        <v>2.51</v>
+      </c>
+      <c r="G5">
+        <v>3.93</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
         <v>0.2</v>
       </c>
-      <c r="F5">
-        <v>0.37</v>
-      </c>
-      <c r="G5">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="H5">
-        <v>0.12</v>
-      </c>
-      <c r="I5">
-        <v>0.62</v>
-      </c>
       <c r="J5">
-        <v>1.83</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FOSA</t>
+          <t>L-PFOS</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.18</v>
+        <v>8.91</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>10.59</v>
       </c>
       <c r="D6">
+        <v>13.75</v>
+      </c>
+      <c r="E6">
+        <v>4.63</v>
+      </c>
+      <c r="F6">
+        <v>6.74</v>
+      </c>
+      <c r="G6">
+        <v>9.720000000000001</v>
+      </c>
+      <c r="H6">
         <v>0.92</v>
       </c>
-      <c r="E6">
-        <v>2.07</v>
-      </c>
-      <c r="F6">
-        <v>2.51</v>
-      </c>
-      <c r="G6">
-        <v>3.93</v>
-      </c>
-      <c r="H6">
-        <v>0.05</v>
-      </c>
       <c r="I6">
-        <v>0.2</v>
+        <v>1.57</v>
       </c>
       <c r="J6">
-        <v>0.45</v>
+        <v>2.97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>L-PFOS</t>
+          <t>PFDA</t>
         </is>
       </c>
       <c r="B7">
-        <v>8.91</v>
+        <v>1.1</v>
       </c>
       <c r="C7">
-        <v>10.59</v>
+        <v>1.57</v>
       </c>
       <c r="D7">
-        <v>13.75</v>
+        <v>2.15</v>
       </c>
       <c r="E7">
-        <v>4.63</v>
+        <v>0.31</v>
       </c>
       <c r="F7">
-        <v>6.74</v>
+        <v>1.01</v>
       </c>
       <c r="G7">
-        <v>9.720000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="H7">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="I7">
-        <v>1.57</v>
+        <v>1.55</v>
       </c>
       <c r="J7">
-        <v>2.97</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PFDA</t>
+          <t>PFDoDA</t>
         </is>
       </c>
       <c r="B8">
-        <v>1.1</v>
+        <v>0.66</v>
       </c>
       <c r="C8">
-        <v>1.57</v>
+        <v>1.01</v>
       </c>
       <c r="D8">
-        <v>2.15</v>
+        <v>1.24</v>
       </c>
       <c r="E8">
-        <v>0.31</v>
+        <v>0.55</v>
       </c>
       <c r="F8">
-        <v>1.01</v>
+        <v>0.72</v>
       </c>
       <c r="G8">
-        <v>1.3</v>
+        <v>0.97</v>
       </c>
       <c r="H8">
-        <v>0.84</v>
+        <v>0.68</v>
       </c>
       <c r="I8">
-        <v>1.55</v>
+        <v>1.4</v>
       </c>
       <c r="J8">
-        <v>6.99</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PFDoDA</t>
+          <t>PFNA</t>
         </is>
       </c>
       <c r="B9">
-        <v>0.66</v>
+        <v>0.89</v>
       </c>
       <c r="C9">
-        <v>1.01</v>
+        <v>1.14</v>
       </c>
       <c r="D9">
-        <v>1.24</v>
+        <v>1.8</v>
       </c>
       <c r="E9">
-        <v>0.55</v>
+        <v>0.42</v>
       </c>
       <c r="F9">
-        <v>0.72</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G9">
-        <v>0.97</v>
+        <v>0.89</v>
       </c>
       <c r="H9">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1.4</v>
+        <v>2.03</v>
       </c>
       <c r="J9">
-        <v>2.24</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PFNA</t>
+          <t>PFTeDA</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1.14</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1.8</v>
+        <v>0.63</v>
       </c>
       <c r="E10">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.5600000000000001</v>
+        <v>0.48</v>
       </c>
       <c r="G10">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>2.03</v>
-      </c>
-      <c r="J10">
-        <v>4.31</v>
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Inf</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PFPeA</t>
+          <t>PFTrDA</t>
         </is>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="C11">
-        <v>0.58</v>
+        <v>0.41</v>
       </c>
       <c r="D11">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="G11">
-        <v>0.65</v>
+        <v>0.28</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
+        <v>0.84</v>
+      </c>
+      <c r="I11">
+        <v>2.28</v>
+      </c>
+      <c r="J11">
+        <v>3.54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PFTeDA</t>
+          <t>PFUnDA</t>
         </is>
       </c>
       <c r="B12">
@@ -766,16 +764,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.63</v>
+        <v>0.19</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="F12">
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
       <c r="G12">
-        <v>0.88</v>
+        <v>0.37</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -783,112 +781,42 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
+      <c r="J12">
+        <v>1.67</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PFTrDA</t>
+          <t>sumPFAS</t>
         </is>
       </c>
       <c r="B13">
-        <v>0.24</v>
+        <v>14.21</v>
       </c>
       <c r="C13">
-        <v>0.41</v>
+        <v>17.03</v>
       </c>
       <c r="D13">
-        <v>0.45</v>
+        <v>25.71</v>
       </c>
       <c r="E13">
-        <v>0.13</v>
+        <v>10.58</v>
       </c>
       <c r="F13">
-        <v>0.18</v>
+        <v>15.1</v>
       </c>
       <c r="G13">
-        <v>0.28</v>
+        <v>18.7</v>
       </c>
       <c r="H13">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="I13">
-        <v>2.28</v>
+        <v>1.13</v>
       </c>
       <c r="J13">
-        <v>3.54</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>PFUnDA</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.19</v>
-      </c>
-      <c r="E14">
-        <v>0.11</v>
-      </c>
-      <c r="F14">
-        <v>0.24</v>
-      </c>
-      <c r="G14">
-        <v>0.37</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>sumPFAS</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>15.14</v>
-      </c>
-      <c r="C15">
-        <v>17.52</v>
-      </c>
-      <c r="D15">
-        <v>25.71</v>
-      </c>
-      <c r="E15">
-        <v>12.79</v>
-      </c>
-      <c r="F15">
-        <v>17.67</v>
-      </c>
-      <c r="G15">
-        <v>25.43</v>
-      </c>
-      <c r="H15">
-        <v>0.6</v>
-      </c>
-      <c r="I15">
-        <v>0.99</v>
-      </c>
-      <c r="J15">
-        <v>2.01</v>
+        <v>2.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>